<commit_message>
Added Webservice links for Prod server
Added both links for local and production servers.
</commit_message>
<xml_diff>
--- a/WebServices.xlsx
+++ b/WebServices.xlsx
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
-  <si>
-    <t>Man Market WebServices</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>REST Protocol</t>
   </si>
   <si>
-    <t>http://localhost:8080/MMarketWebService/getAllPatronLoginHist</t>
-  </si>
-  <si>
-    <t>http://localhost:8080/MMarketWebService/</t>
-  </si>
-  <si>
     <t>http://localhost:8080/MMarketWebService/getPatronLoginHistByPatronId/{patronId}</t>
   </si>
   <si>
@@ -60,6 +51,36 @@
   </si>
   <si>
     <t>PUT</t>
+  </si>
+  <si>
+    <t>http://localhost:8080/MMarketWebServicegetAllPatronLoginHist</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/</t>
+  </si>
+  <si>
+    <t>Man Market WebServices - LOCAL SERVER</t>
+  </si>
+  <si>
+    <t>Man Market WebServices - PRODUCTION SERVER</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/getPatronLoginHistByHistId/{histId}</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/getPatronLoginHistByPatronId/{patronId}</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/getPatronLoginHistByDateRange/{startDate}/{endDate}</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/updatePatronById/{patronId}/{lastLoginDate}</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/addPatronLoginHistRec/{patronId}/{lastLoginDate}</t>
+  </si>
+  <si>
+    <t>http://apps-imeetem.com/MMarketWebService/getAllPatronLoginHist</t>
   </si>
 </sst>
 </file>
@@ -124,10 +145,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -443,123 +462,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="91.140625" customWidth="1"/>
+    <col min="2" max="2" width="97.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId8"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>